<commit_message>
develop loop that moves through GC files
</commit_message>
<xml_diff>
--- a/GC-Data-Raw-R/GC-Data-standardizedfilenames/runsheets-standardizedfilenames/runsheet_20131105_BB.xlsx
+++ b/GC-Data-Raw-R/GC-Data-standardizedfilenames/runsheets-standardizedfilenames/runsheet_20131105_BB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18560" yWindow="280" windowWidth="13680" windowHeight="17820" tabRatio="500"/>
+    <workbookView xWindow="6160" yWindow="280" windowWidth="26080" windowHeight="17820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -286,18 +286,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -585,8 +579,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="271">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1190,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1211,10 +1205,10 @@
       <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
@@ -1243,10 +1237,10 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F2" t="s">
@@ -1275,10 +1269,10 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
@@ -1307,10 +1301,10 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
@@ -1339,10 +1333,10 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F5" t="s">
@@ -1371,10 +1365,10 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F6" t="s">
@@ -1403,10 +1397,10 @@
       <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
@@ -1435,10 +1429,10 @@
       <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F8" t="s">
@@ -1467,10 +1461,10 @@
       <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F9" t="s">
@@ -1499,10 +1493,10 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F10" t="s">
@@ -1531,10 +1525,10 @@
       <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F11" t="s">
@@ -1563,10 +1557,10 @@
       <c r="C12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F12" t="str">
@@ -1586,7 +1580,7 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12:J21" si="4">I12^2</f>
+        <f t="shared" ref="J12:J59" si="4">I12^2</f>
         <v>0</v>
       </c>
     </row>
@@ -1600,10 +1594,10 @@
       <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F13" t="str">
@@ -1637,10 +1631,10 @@
       <c r="C14" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F14" t="str">
@@ -1674,10 +1668,10 @@
       <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F15" t="str">
@@ -1711,10 +1705,10 @@
       <c r="C16" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F16" t="str">
@@ -1748,10 +1742,10 @@
       <c r="C17" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F17" t="str">
@@ -1785,10 +1779,10 @@
       <c r="C18" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F18" t="str">
@@ -1822,10 +1816,10 @@
       <c r="C19" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F19" t="str">
@@ -1859,10 +1853,10 @@
       <c r="C20" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F20" t="str">
@@ -1896,10 +1890,10 @@
       <c r="C21" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F21" t="str">
@@ -1933,10 +1927,10 @@
       <c r="C22" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="D22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F22" t="str">
@@ -1948,16 +1942,16 @@
         <v>S</v>
       </c>
       <c r="H22" t="str">
-        <f t="shared" ref="H22:H43" si="7">MID(E22,4,2)</f>
-        <v>C-</v>
+        <f>MID(E22,4,1)</f>
+        <v>C</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" ref="I22:I43" si="8">MID(E22,11,2)</f>
-        <v>0</v>
+        <f t="shared" ref="I22:I59" si="7">MID(E22,10,2)</f>
+        <v>20</v>
       </c>
       <c r="J22">
-        <f t="shared" ref="J22:J44" si="9">I22^2</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>400</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1970,10 +1964,10 @@
       <c r="C23" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="D23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F23" t="str">
@@ -1985,16 +1979,16 @@
         <v>S</v>
       </c>
       <c r="H23" t="str">
-        <f t="shared" si="7"/>
-        <v>C-</v>
+        <f t="shared" ref="H23:H43" si="8">MID(E23,4,1)</f>
+        <v>C</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>30</v>
       </c>
       <c r="J23">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>900</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -2007,10 +2001,10 @@
       <c r="C24" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="D24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F24" t="str">
@@ -2022,16 +2016,16 @@
         <v>S</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" si="7"/>
-        <v>D-</v>
+        <f t="shared" si="8"/>
+        <v>D</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J24" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2044,10 +2038,10 @@
       <c r="C25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="D25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F25" t="str">
@@ -2059,16 +2053,16 @@
         <v>S</v>
       </c>
       <c r="H25" t="str">
-        <f t="shared" si="7"/>
-        <v>D-</v>
+        <f t="shared" si="8"/>
+        <v>D</v>
       </c>
       <c r="I25" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="J25">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -2081,10 +2075,10 @@
       <c r="C26" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="D26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F26" t="str">
@@ -2096,16 +2090,16 @@
         <v>S</v>
       </c>
       <c r="H26" t="str">
-        <f t="shared" si="7"/>
-        <v>D-</v>
+        <f t="shared" si="8"/>
+        <v>D</v>
       </c>
       <c r="I26" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
       <c r="J26">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>400</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2118,10 +2112,10 @@
       <c r="C27" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="D27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F27" t="str">
@@ -2133,16 +2127,16 @@
         <v>S</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" si="7"/>
-        <v>D-</v>
+        <f t="shared" si="8"/>
+        <v>D</v>
       </c>
       <c r="I27" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>30</v>
       </c>
       <c r="J27">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>900</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2155,10 +2149,10 @@
       <c r="C28" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="D28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F28" t="str">
@@ -2170,16 +2164,16 @@
         <v>S</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="7"/>
-        <v>E-</v>
+        <f t="shared" si="8"/>
+        <v>E</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J28" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2192,10 +2186,10 @@
       <c r="C29" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="D29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F29" t="str">
@@ -2207,16 +2201,16 @@
         <v>S</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="7"/>
-        <v>E-</v>
+        <f t="shared" si="8"/>
+        <v>E</v>
       </c>
       <c r="I29" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="J29">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2229,10 +2223,10 @@
       <c r="C30" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="D30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F30" t="str">
@@ -2244,16 +2238,16 @@
         <v>S</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="7"/>
-        <v>E-</v>
+        <f t="shared" si="8"/>
+        <v>E</v>
       </c>
       <c r="I30" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
       <c r="J30">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>400</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2266,10 +2260,10 @@
       <c r="C31" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="3" t="s">
+      <c r="D31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F31" t="str">
@@ -2281,16 +2275,16 @@
         <v>S</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="7"/>
-        <v>E-</v>
+        <f t="shared" si="8"/>
+        <v>E</v>
       </c>
       <c r="I31" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>30</v>
       </c>
       <c r="J31">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>900</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2303,10 +2297,10 @@
       <c r="C32" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="D32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>45</v>
       </c>
       <c r="F32" t="str">
@@ -2318,16 +2312,16 @@
         <v>S</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="7"/>
-        <v>A-</v>
+        <f t="shared" si="8"/>
+        <v>A</v>
       </c>
       <c r="I32" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J32" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2340,10 +2334,10 @@
       <c r="C33" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="3" t="s">
+      <c r="D33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F33" t="str">
@@ -2355,16 +2349,16 @@
         <v>S</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="7"/>
-        <v>A-</v>
+        <f t="shared" si="8"/>
+        <v>A</v>
       </c>
       <c r="I33" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="J33">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2377,10 +2371,10 @@
       <c r="C34" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="3" t="s">
+      <c r="D34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F34" t="str">
@@ -2392,16 +2386,16 @@
         <v>S</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="7"/>
-        <v>A-</v>
+        <f t="shared" si="8"/>
+        <v>A</v>
       </c>
       <c r="I34" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
       <c r="J34">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>400</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2414,10 +2408,10 @@
       <c r="C35" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="D35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F35" t="str">
@@ -2429,16 +2423,16 @@
         <v>S</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="7"/>
-        <v>A-</v>
+        <f t="shared" si="8"/>
+        <v>A</v>
       </c>
       <c r="I35" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>30</v>
       </c>
       <c r="J35">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>900</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2451,10 +2445,10 @@
       <c r="C36" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="D36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F36" t="str">
@@ -2466,16 +2460,16 @@
         <v>S</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="7"/>
-        <v>B-</v>
+        <f t="shared" si="8"/>
+        <v>B</v>
       </c>
       <c r="I36" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J36" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2488,10 +2482,10 @@
       <c r="C37" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="D37" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F37" t="str">
@@ -2503,16 +2497,16 @@
         <v>S</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="7"/>
-        <v>B-</v>
+        <f t="shared" si="8"/>
+        <v>B</v>
       </c>
       <c r="I37" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="J37">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2525,10 +2519,10 @@
       <c r="C38" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="D38" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F38" t="str">
@@ -2540,16 +2534,16 @@
         <v>S</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="7"/>
-        <v>B-</v>
+        <f t="shared" si="8"/>
+        <v>B</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
       <c r="J38">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>400</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2562,10 +2556,10 @@
       <c r="C39" t="s">
         <v>10</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="3" t="s">
+      <c r="D39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F39" t="str">
@@ -2577,16 +2571,16 @@
         <v>S</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="7"/>
-        <v>B-</v>
+        <f t="shared" si="8"/>
+        <v>B</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>30</v>
       </c>
       <c r="J39">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>900</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2599,10 +2593,10 @@
       <c r="C40" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" s="3" t="s">
+      <c r="D40" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F40" t="str">
@@ -2614,16 +2608,16 @@
         <v>S</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="7"/>
-        <v>C-</v>
+        <f t="shared" si="8"/>
+        <v>C</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J40" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2636,10 +2630,10 @@
       <c r="C41" t="s">
         <v>10</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="D41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F41" t="str">
@@ -2651,16 +2645,16 @@
         <v>S</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="7"/>
-        <v>C-</v>
+        <f t="shared" si="8"/>
+        <v>C</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="J41">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2673,10 +2667,10 @@
       <c r="C42" t="s">
         <v>10</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="3" t="s">
+      <c r="D42" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F42" t="str">
@@ -2688,16 +2682,16 @@
         <v>M</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="7"/>
-        <v>C-</v>
+        <f t="shared" si="8"/>
+        <v>C</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
       <c r="J42">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>400</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2710,10 +2704,10 @@
       <c r="C43" t="s">
         <v>10</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="D43" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F43" t="str">
@@ -2725,16 +2719,16 @@
         <v>M</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="7"/>
-        <v>C-</v>
+        <f t="shared" si="8"/>
+        <v>C</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>30</v>
       </c>
       <c r="J43">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>900</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2747,10 +2741,10 @@
       <c r="C44" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E44" s="3" t="s">
+      <c r="D44" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F44" t="str">
@@ -2762,15 +2756,15 @@
         <v>M</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" ref="H44" si="10">MID(E44,4,1)</f>
+        <f>MID(E44,4,1)</f>
         <v>D</v>
       </c>
       <c r="I44" t="str">
-        <f t="shared" ref="I44" si="11">MID(E44,10,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2784,30 +2778,30 @@
       <c r="C45" t="s">
         <v>10</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E45" s="3" t="s">
+      <c r="D45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" ref="F45:F63" si="12">LEFT(E45,2)</f>
+        <f t="shared" ref="F45:F63" si="9">LEFT(E45,2)</f>
         <v>M3</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" ref="G45:G63" si="13">LEFT(F45,1)</f>
+        <f t="shared" ref="G45:G63" si="10">LEFT(F45,1)</f>
         <v>M</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" ref="H45:H63" si="14">MID(E45,4,1)</f>
+        <f t="shared" ref="H45:H63" si="11">MID(E45,4,1)</f>
         <v>D</v>
       </c>
       <c r="I45" t="str">
-        <f t="shared" ref="I45:I63" si="15">MID(E45,10,2)</f>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J45">
-        <f t="shared" ref="J45:J63" si="16">I45^2</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
     </row>
@@ -2821,30 +2815,30 @@
       <c r="C46" t="s">
         <v>10</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E46" s="3" t="s">
+      <c r="D46" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>M3</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>D</v>
       </c>
       <c r="I46" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="J46">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
     </row>
@@ -2858,30 +2852,30 @@
       <c r="C47" t="s">
         <v>10</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E47" s="3" t="s">
+      <c r="D47" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>M3</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>D</v>
       </c>
       <c r="I47" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="J47">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
     </row>
@@ -2895,30 +2889,30 @@
       <c r="C48" t="s">
         <v>10</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E48" s="3" t="s">
+      <c r="D48" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>61</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>M3</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>E</v>
       </c>
       <c r="I48" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2932,30 +2926,30 @@
       <c r="C49" t="s">
         <v>10</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" s="3" t="s">
+      <c r="D49" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>62</v>
       </c>
       <c r="F49" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>M3</v>
       </c>
       <c r="G49" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="H49" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>E</v>
       </c>
       <c r="I49" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
     </row>
@@ -2969,30 +2963,30 @@
       <c r="C50" t="s">
         <v>10</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E50" s="3" t="s">
+      <c r="D50" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F50" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>M3</v>
       </c>
       <c r="G50" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="H50" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>E</v>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="J50">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
     </row>
@@ -3006,30 +3000,30 @@
       <c r="C51" t="s">
         <v>10</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E51" s="3" t="s">
+      <c r="D51" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>M3</v>
       </c>
       <c r="G51" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="H51" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>E</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="J51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
     </row>
@@ -3043,30 +3037,30 @@
       <c r="C52" t="s">
         <v>10</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E52" s="3" t="s">
+      <c r="D52" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>M3</v>
       </c>
       <c r="G52" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="H52" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>A</v>
       </c>
       <c r="I52" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J52">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3080,30 +3074,30 @@
       <c r="C53" t="s">
         <v>10</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E53" s="3" t="s">
+      <c r="D53" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F53" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>M3</v>
       </c>
       <c r="G53" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="H53" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>A</v>
       </c>
       <c r="I53" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J53">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
     </row>
@@ -3117,18 +3111,18 @@
       <c r="C54" t="s">
         <v>10</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E54" s="3" t="s">
+      <c r="D54" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F54" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>M3</v>
       </c>
       <c r="G54" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="H54" t="str">
@@ -3136,11 +3130,11 @@
         <v>A</v>
       </c>
       <c r="I54" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="J54">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
     </row>
@@ -3154,30 +3148,30 @@
       <c r="C55" t="s">
         <v>10</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E55" s="3" t="s">
+      <c r="D55" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F55" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>M3</v>
       </c>
       <c r="G55" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="H55" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>A</v>
       </c>
       <c r="I55" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="J55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
     </row>
@@ -3191,30 +3185,30 @@
       <c r="C56" t="s">
         <v>10</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E56" s="3" t="s">
+      <c r="D56" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F56" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>M3</v>
       </c>
       <c r="G56" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="H56" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>B</v>
       </c>
       <c r="I56" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3228,30 +3222,30 @@
       <c r="C57" t="s">
         <v>10</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E57" s="3" t="s">
+      <c r="D57" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F57" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>M3</v>
       </c>
       <c r="G57" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="H57" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>B</v>
       </c>
       <c r="I57" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
     </row>
@@ -3265,30 +3259,30 @@
       <c r="C58" t="s">
         <v>10</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E58" s="3" t="s">
+      <c r="D58" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F58" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>M3</v>
       </c>
       <c r="G58" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="H58" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>B</v>
       </c>
       <c r="I58" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="J58">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
     </row>
@@ -3302,30 +3296,30 @@
       <c r="C59" t="s">
         <v>10</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E59" s="3" t="s">
+      <c r="D59" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F59" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>M3</v>
       </c>
       <c r="G59" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="H59" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>B</v>
       </c>
       <c r="I59" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="J59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
     </row>
@@ -3339,30 +3333,30 @@
       <c r="C60" t="s">
         <v>10</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E60" s="3" t="s">
+      <c r="D60" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>M3</v>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="H60" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>C</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="I45:I63" si="12">MID(E60,10,2)</f>
         <v>0</v>
       </c>
       <c r="J60">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="J45:J63" si="13">I60^2</f>
         <v>0</v>
       </c>
     </row>
@@ -3376,30 +3370,30 @@
       <c r="C61" t="s">
         <v>10</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E61" s="3" t="s">
+      <c r="D61" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F61" t="str">
+        <f t="shared" si="9"/>
+        <v>M3</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="10"/>
+        <v>M</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="11"/>
+        <v>C</v>
+      </c>
+      <c r="I61" t="str">
         <f t="shared" si="12"/>
-        <v>M3</v>
-      </c>
-      <c r="G61" t="str">
+        <v>10</v>
+      </c>
+      <c r="J61">
         <f t="shared" si="13"/>
-        <v>M</v>
-      </c>
-      <c r="H61" t="str">
-        <f t="shared" si="14"/>
-        <v>C</v>
-      </c>
-      <c r="I61" t="str">
-        <f t="shared" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="J61">
-        <f t="shared" si="16"/>
         <v>100</v>
       </c>
     </row>
@@ -3420,23 +3414,23 @@
         <v>22</v>
       </c>
       <c r="F62" t="str">
+        <f t="shared" si="9"/>
+        <v>F1</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="10"/>
+        <v>F</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="11"/>
+        <v>A</v>
+      </c>
+      <c r="I62" t="str">
         <f t="shared" si="12"/>
-        <v>F1</v>
-      </c>
-      <c r="G62" t="str">
+        <v>20</v>
+      </c>
+      <c r="J62">
         <f t="shared" si="13"/>
-        <v>F</v>
-      </c>
-      <c r="H62" t="str">
-        <f t="shared" si="14"/>
-        <v>A</v>
-      </c>
-      <c r="I62" t="str">
-        <f t="shared" si="15"/>
-        <v>20</v>
-      </c>
-      <c r="J62">
-        <f t="shared" si="16"/>
         <v>400</v>
       </c>
     </row>
@@ -3457,23 +3451,23 @@
         <v>23</v>
       </c>
       <c r="F63" t="str">
+        <f t="shared" si="9"/>
+        <v>F1</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="10"/>
+        <v>F</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="11"/>
+        <v>A</v>
+      </c>
+      <c r="I63" t="str">
         <f t="shared" si="12"/>
-        <v>F1</v>
-      </c>
-      <c r="G63" t="str">
+        <v>30</v>
+      </c>
+      <c r="J63">
         <f t="shared" si="13"/>
-        <v>F</v>
-      </c>
-      <c r="H63" t="str">
-        <f t="shared" si="14"/>
-        <v>A</v>
-      </c>
-      <c r="I63" t="str">
-        <f t="shared" si="15"/>
-        <v>30</v>
-      </c>
-      <c r="J63">
-        <f t="shared" si="16"/>
         <v>900</v>
       </c>
     </row>

</xml_diff>